<commit_message>
Change to new version
</commit_message>
<xml_diff>
--- a/TestFile_HW1/Password vs Hashed.xlsx
+++ b/TestFile_HW1/Password vs Hashed.xlsx
@@ -26,64 +26,64 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>69meetIng587377</t>
-  </si>
-  <si>
-    <t>CloTHE367764763</t>
-  </si>
-  <si>
-    <t>778063883NATure</t>
-  </si>
-  <si>
-    <t>7522242rELY39</t>
-  </si>
-  <si>
-    <t>920744694dirECtor</t>
-  </si>
-  <si>
-    <t>1synTheSIs16125714</t>
-  </si>
-  <si>
-    <t>12PALTRy9946405</t>
-  </si>
-  <si>
-    <t>egotiSM263912575</t>
-  </si>
-  <si>
-    <t>23424405cOMMOtiON</t>
-  </si>
-  <si>
-    <t>1e98d3e6225d47c98e63a93ae18e424c</t>
-  </si>
-  <si>
-    <t>45c44af3a7b0721b1873378a1305f736</t>
-  </si>
-  <si>
-    <t>843f09d2c610c3d8d9677724e5d4bcef</t>
-  </si>
-  <si>
-    <t>d4b68189f9229b6dc11ccc6047797ce1</t>
-  </si>
-  <si>
-    <t>686a9c23a69f635352c076ac58ba6f7e</t>
-  </si>
-  <si>
-    <t>33bd1d175002211de26e7eaa588427b4</t>
-  </si>
-  <si>
-    <t>06245faf6179f972e10d77ed4aa199d3</t>
-  </si>
-  <si>
-    <t>18329f9867d7e7cb3e246012f0509769</t>
-  </si>
-  <si>
-    <t>998dba5755b89dbb3ce9c098f5e4cdb2</t>
-  </si>
-  <si>
-    <t>922924701STUBbORn</t>
-  </si>
-  <si>
-    <t>1017fb2f29559b07fc41e3e75e9c5626</t>
+    <t>81ea785a5e780dc106921e3bcd6cbdfb</t>
+  </si>
+  <si>
+    <t>9805wHOlE</t>
+  </si>
+  <si>
+    <t>aeb5c0e7f6f709c49cf81d6ba8791fd8</t>
+  </si>
+  <si>
+    <t>21385AgeNdA</t>
+  </si>
+  <si>
+    <t>869a174703dee3655aebd65402242a81</t>
+  </si>
+  <si>
+    <t>8MiXTuRE5</t>
+  </si>
+  <si>
+    <t>9508d669d383d9526a31cf69dde6bde8</t>
+  </si>
+  <si>
+    <t>6poStER</t>
+  </si>
+  <si>
+    <t>4f108a47880629f180fbc3c0aa2d6fdf</t>
+  </si>
+  <si>
+    <t>sEntiENt13</t>
+  </si>
+  <si>
+    <t>cb6740a300d203fc1d7a9378825c2c2c</t>
+  </si>
+  <si>
+    <t>121654River</t>
+  </si>
+  <si>
+    <t>d804ecf5b670a04dde27c3670f0c1ac8</t>
+  </si>
+  <si>
+    <t>8fIngEr</t>
+  </si>
+  <si>
+    <t>8e33ed543e50821e13ffa7454af27010</t>
+  </si>
+  <si>
+    <t>CONCepT01</t>
+  </si>
+  <si>
+    <t>7f0d170908317ab2abe9cbb1c5448627</t>
+  </si>
+  <si>
+    <t>aNNEx838</t>
+  </si>
+  <si>
+    <t>0a5840d9466c49b1a3a4fe3ff7ae6599</t>
+  </si>
+  <si>
+    <t>25OBEdIENt78</t>
   </si>
 </sst>
 </file>
@@ -145,7 +145,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -450,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -475,94 +477,104 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" t="s">
-        <v>12</v>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" t="s">
-        <v>14</v>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-    </row>
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>